<commit_message>
Mania and Nikolia artciles
</commit_message>
<xml_diff>
--- a/Reviewer_Comments_R_1_23-Dec-2024.xlsx
+++ b/Reviewer_Comments_R_1_23-Dec-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Publications\Article_Empirical_Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAC394D-ED7A-4A18-AD11-0DCD8405A0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6358AB-2351-427F-817B-979C688E4F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="210">
   <si>
     <t>Reviewer 1</t>
   </si>
@@ -2243,12 +2243,68 @@
   <si>
     <t>Point-by-Point</t>
   </si>
+  <si>
+    <t>R-2-13</t>
+  </si>
+  <si>
+    <t>Ref: Nikolai_Matni_2019_REINFORCE_lecture</t>
+  </si>
+  <si>
+    <t>direct policy search, derivative-free, can solve "unconstrained optimization problems through function evaluations."</t>
+  </si>
+  <si>
+    <t>If you can sample efficiently from p(z; theta), then you can run the algorithm on essentially any problem.</t>
+  </si>
+  <si>
+    <t>using a derivative-free optimization method, and can not achieve the same perfor-
+mance as methods that compute actual gradients. This performance gap is exacerbated when the function
+evaluations are noisy. Another drawback to this approach is that our choice of probability distribution can
+lead to high variance of stochastic gradients. High variance requires more samples to be drawn in order to
+_x000C_nd a minima or maxima. In other words, sample complexity increases.</t>
+  </si>
+  <si>
+    <t>Although the approach has a few drawbacks, the simplicity of implementation is often valuable enough to
+justify its use. There are two primary applications of this sort of stochastic search approach in reinforcement
+learning: policy gradient and pure random search.</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Performance is Domain specific</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nikolai_Matni_2019</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: It is difficult to say which approach is better without selecting a specific problem to which to apply them</t>
+    </r>
+  </si>
+  <si>
+    <t>mania2018: &gt;&gt; Simple random search provides a competitive approach to reinforcement learning</t>
+  </si>
+  <si>
+    <t>Computationally, our random search algorithm is at least 15 times more e_x000E_cient than the fastest competing model-free methods on these benchmarks.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="52" x14ac:knownFonts="1">
+  <fonts count="57" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2606,6 +2662,41 @@
       <name val="Aptos Display"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -2664,12 +2755,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFB0EED0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2689,6 +2774,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3040,7 +3131,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3343,9 +3434,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -3379,7 +3467,7 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3412,25 +3500,25 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
@@ -3447,104 +3535,128 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="53" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="54" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="55" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4782,9 +4894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816F3457-95CC-4A5E-96D0-1EA42C9E78DF}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4811,32 +4923,32 @@
       <c r="D1" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="119" t="s">
+      <c r="E1" s="118" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="119" t="s">
+      <c r="F1" s="118" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="119" t="s">
+      <c r="G1" s="118" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="120" t="s">
+      <c r="H1" s="119" t="s">
         <v>135</v>
       </c>
       <c r="I1" s="88"/>
-      <c r="J1" s="127" t="s">
+      <c r="J1" s="126" t="s">
         <v>161</v>
       </c>
-      <c r="K1" s="128" t="s">
+      <c r="K1" s="127" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="128" t="s">
+      <c r="L1" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="128" t="s">
+      <c r="M1" s="127" t="s">
         <v>130</v>
       </c>
-      <c r="N1" s="107" t="s">
+      <c r="N1" s="106" t="s">
         <v>139</v>
       </c>
       <c r="O1" s="88"/>
@@ -4861,20 +4973,20 @@
         <v>130</v>
       </c>
       <c r="G2" s="61"/>
-      <c r="H2" s="121"/>
+      <c r="H2" s="120"/>
       <c r="I2" s="89"/>
-      <c r="J2" s="129" t="s">
+      <c r="J2" s="128" t="s">
         <v>129</v>
       </c>
-      <c r="K2" s="108">
+      <c r="K2" s="107">
         <f>COUNTA(C2)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108">
+      <c r="L2" s="107"/>
+      <c r="M2" s="107">
         <v>1</v>
       </c>
-      <c r="N2" s="109">
+      <c r="N2" s="108">
         <f>K2-M2</f>
         <v>0</v>
       </c>
@@ -4898,22 +5010,24 @@
       </c>
       <c r="F3" s="86"/>
       <c r="G3" s="86"/>
-      <c r="H3" s="122"/>
+      <c r="H3" s="121"/>
       <c r="I3" s="89"/>
-      <c r="J3" s="130" t="s">
+      <c r="J3" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="108">
+      <c r="K3" s="107">
         <f>COUNTA(C3:C11)</f>
         <v>9</v>
       </c>
-      <c r="L3" s="108">
-        <v>1</v>
-      </c>
-      <c r="M3" s="108">
+      <c r="L3" s="107">
+        <f>COUNTIF($E$3:$E$11,"WIP")</f>
+        <v>2</v>
+      </c>
+      <c r="M3" s="107">
+        <f>COUNTIF($E$3:$E$11,"Done")</f>
         <v>3</v>
       </c>
-      <c r="N3" s="109">
+      <c r="N3" s="108">
         <f t="shared" ref="N3:N4" si="0">K3-M3</f>
         <v>6</v>
       </c>
@@ -4937,25 +5051,27 @@
       </c>
       <c r="F4" s="86"/>
       <c r="G4" s="86"/>
-      <c r="H4" s="122" t="s">
+      <c r="H4" s="121" t="s">
         <v>160</v>
       </c>
       <c r="I4" s="89"/>
-      <c r="J4" s="131" t="s">
+      <c r="J4" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="110">
+      <c r="K4" s="109">
         <f>COUNTA(C12:C23)</f>
         <v>12</v>
       </c>
-      <c r="L4" s="110">
+      <c r="L4" s="109">
+        <f>COUNTIF($E$12:$E$23,"WIP")</f>
         <v>2</v>
       </c>
-      <c r="M4" s="110">
+      <c r="M4" s="109">
+        <f>COUNTIF($E$12:$E$23,"Done")</f>
         <v>3</v>
       </c>
-      <c r="N4" s="111">
-        <f t="shared" si="0"/>
+      <c r="N4" s="110">
+        <f>K4-M4</f>
         <v>9</v>
       </c>
       <c r="O4" s="89"/>
@@ -4976,24 +5092,24 @@
       </c>
       <c r="F5" s="86"/>
       <c r="G5" s="86"/>
-      <c r="H5" s="122" t="s">
+      <c r="H5" s="121" t="s">
         <v>127</v>
       </c>
       <c r="I5" s="89"/>
       <c r="J5" s="91"/>
-      <c r="K5" s="112">
+      <c r="K5" s="111">
         <f t="shared" ref="K5:L5" si="1">SUM(K2:K4)</f>
         <v>22</v>
       </c>
-      <c r="L5" s="112">
+      <c r="L5" s="111">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="M5" s="112">
+        <v>4</v>
+      </c>
+      <c r="M5" s="177">
         <f>SUM(M2:M4)</f>
         <v>7</v>
       </c>
-      <c r="N5" s="113">
+      <c r="N5" s="112">
         <f>SUM(N2:N4)</f>
         <v>15</v>
       </c>
@@ -5017,21 +5133,21 @@
       </c>
       <c r="F6" s="86"/>
       <c r="G6" s="86"/>
-      <c r="H6" s="122" t="s">
+      <c r="H6" s="121" t="s">
         <v>151</v>
       </c>
       <c r="I6" s="89"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="114">
+      <c r="J6" s="173"/>
+      <c r="K6" s="173"/>
+      <c r="L6" s="174">
         <f>L5/$K$5</f>
-        <v>0.13636363636363635</v>
-      </c>
-      <c r="M6" s="114">
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="M6" s="175">
         <f>M5/$K$5</f>
         <v>0.31818181818181818</v>
       </c>
-      <c r="N6" s="114">
+      <c r="N6" s="176">
         <f>N5/$K$5</f>
         <v>0.68181818181818177</v>
       </c>
@@ -5055,21 +5171,21 @@
       </c>
       <c r="F7" s="86"/>
       <c r="G7" s="86"/>
-      <c r="H7" s="122" t="s">
+      <c r="H7" s="121" t="s">
         <v>194</v>
       </c>
       <c r="I7" s="89"/>
-      <c r="J7" s="105" t="s">
+      <c r="J7" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="K7" s="140">
+      <c r="K7" s="156">
         <v>45657</v>
       </c>
-      <c r="L7" s="140"/>
+      <c r="L7" s="156"/>
       <c r="M7" s="89"/>
-      <c r="N7" s="114">
+      <c r="N7" s="113">
         <f>(M5+L5)/K5</f>
-        <v>0.45454545454545453</v>
+        <v>0.5</v>
       </c>
       <c r="O7" s="89" t="s">
         <v>169</v>
@@ -5088,21 +5204,21 @@
       <c r="D8" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="81" t="s">
-        <v>104</v>
+      <c r="E8" s="172" t="s">
+        <v>34</v>
       </c>
       <c r="F8" s="86"/>
       <c r="G8" s="86"/>
-      <c r="H8" s="122"/>
+      <c r="H8" s="121"/>
       <c r="I8" s="89"/>
-      <c r="J8" s="105" t="s">
+      <c r="J8" s="104" t="s">
         <v>132</v>
       </c>
-      <c r="K8" s="140">
+      <c r="K8" s="156">
         <f ca="1">TODAY()</f>
         <v>45649</v>
       </c>
-      <c r="L8" s="140"/>
+      <c r="L8" s="156"/>
       <c r="M8" s="89"/>
       <c r="N8" s="89"/>
       <c r="O8" s="89"/>
@@ -5118,23 +5234,23 @@
       <c r="D9" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="104" t="s">
+      <c r="E9" s="172" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="86"/>
       <c r="G9" s="86"/>
-      <c r="H9" s="122" t="s">
+      <c r="H9" s="121" t="s">
         <v>149</v>
       </c>
       <c r="I9" s="89"/>
-      <c r="J9" s="105" t="s">
+      <c r="J9" s="104" t="s">
         <v>96</v>
       </c>
       <c r="K9" s="89">
         <f ca="1">K7-K8-1</f>
         <v>7</v>
       </c>
-      <c r="L9" s="106"/>
+      <c r="L9" s="105"/>
       <c r="M9" s="89"/>
       <c r="N9" s="89"/>
       <c r="O9" s="89"/>
@@ -5157,7 +5273,7 @@
       </c>
       <c r="F10" s="92"/>
       <c r="G10" s="92"/>
-      <c r="H10" s="123" t="s">
+      <c r="H10" s="122" t="s">
         <v>150</v>
       </c>
       <c r="I10" s="89"/>
@@ -5179,12 +5295,12 @@
       <c r="D11" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="E11" s="156" t="s">
+      <c r="E11" s="139" t="s">
         <v>195</v>
       </c>
       <c r="F11" s="87"/>
       <c r="G11" s="87"/>
-      <c r="H11" s="124"/>
+      <c r="H11" s="123"/>
       <c r="I11" s="89"/>
       <c r="J11" s="89"/>
       <c r="K11" s="89"/>
@@ -5211,21 +5327,21 @@
       </c>
       <c r="F12" s="86"/>
       <c r="G12" s="86"/>
-      <c r="H12" s="122"/>
+      <c r="H12" s="121"/>
       <c r="I12" s="89"/>
-      <c r="J12" s="160" t="s">
+      <c r="J12" s="143" t="s">
         <v>162</v>
       </c>
-      <c r="K12" s="161" t="s">
+      <c r="K12" s="144" t="s">
         <v>89</v>
       </c>
-      <c r="L12" s="161" t="s">
+      <c r="L12" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="161" t="s">
+      <c r="M12" s="144" t="s">
         <v>130</v>
       </c>
-      <c r="N12" s="162" t="s">
+      <c r="N12" s="145" t="s">
         <v>139</v>
       </c>
       <c r="O12" s="89"/>
@@ -5248,15 +5364,15 @@
       </c>
       <c r="F13" s="86"/>
       <c r="G13" s="86"/>
-      <c r="H13" s="122"/>
+      <c r="H13" s="121"/>
       <c r="I13" s="89"/>
-      <c r="J13" s="163" t="s">
+      <c r="J13" s="146" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="157"/>
-      <c r="L13" s="157"/>
-      <c r="M13" s="157"/>
-      <c r="N13" s="164"/>
+      <c r="K13" s="140"/>
+      <c r="L13" s="140"/>
+      <c r="M13" s="140"/>
+      <c r="N13" s="147"/>
       <c r="O13" s="89"/>
     </row>
     <row r="14" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5275,15 +5391,17 @@
       </c>
       <c r="F14" s="86"/>
       <c r="G14" s="86"/>
-      <c r="H14" s="122"/>
+      <c r="H14" s="121" t="s">
+        <v>201</v>
+      </c>
       <c r="I14" s="89"/>
-      <c r="J14" s="165" t="s">
+      <c r="J14" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="157"/>
-      <c r="L14" s="157"/>
-      <c r="M14" s="157"/>
-      <c r="N14" s="164"/>
+      <c r="K14" s="140"/>
+      <c r="L14" s="140"/>
+      <c r="M14" s="140"/>
+      <c r="N14" s="147"/>
       <c r="O14" s="89"/>
     </row>
     <row r="15" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5297,20 +5415,20 @@
       <c r="D15" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="104" t="s">
+      <c r="E15" s="172" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="86"/>
       <c r="G15" s="86"/>
-      <c r="H15" s="122"/>
+      <c r="H15" s="121"/>
       <c r="I15" s="89"/>
-      <c r="J15" s="167" t="s">
+      <c r="J15" s="150" t="s">
         <v>59</v>
       </c>
-      <c r="K15" s="168"/>
-      <c r="L15" s="168"/>
-      <c r="M15" s="168"/>
-      <c r="N15" s="169"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="151"/>
+      <c r="M15" s="151"/>
+      <c r="N15" s="152"/>
       <c r="O15" s="89"/>
     </row>
     <row r="16" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5331,22 +5449,22 @@
       </c>
       <c r="F16" s="86"/>
       <c r="G16" s="86"/>
-      <c r="H16" s="122"/>
+      <c r="H16" s="121"/>
       <c r="I16" s="89"/>
-      <c r="J16" s="170"/>
-      <c r="K16" s="171">
+      <c r="J16" s="153"/>
+      <c r="K16" s="154">
         <f t="shared" ref="K16" si="2">SUM(K13:K15)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="171">
+      <c r="L16" s="154">
         <f t="shared" ref="L16" si="3">SUM(L13:L15)</f>
         <v>0</v>
       </c>
-      <c r="M16" s="171">
+      <c r="M16" s="154">
         <f>SUM(M13:M15)</f>
         <v>0</v>
       </c>
-      <c r="N16" s="172">
+      <c r="N16" s="155">
         <f>SUM(N13:N15)</f>
         <v>0</v>
       </c>
@@ -5370,15 +5488,15 @@
       </c>
       <c r="F17" s="85"/>
       <c r="G17" s="85"/>
-      <c r="H17" s="125" t="s">
+      <c r="H17" s="124" t="s">
         <v>128</v>
       </c>
       <c r="I17" s="89"/>
-      <c r="J17" s="158"/>
-      <c r="K17" s="158"/>
-      <c r="L17" s="159"/>
-      <c r="M17" s="159"/>
-      <c r="N17" s="159"/>
+      <c r="J17" s="141"/>
+      <c r="K17" s="141"/>
+      <c r="L17" s="142"/>
+      <c r="M17" s="142"/>
+      <c r="N17" s="142"/>
       <c r="O17" s="89"/>
     </row>
     <row r="18" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5394,28 +5512,28 @@
       <c r="D18" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="104" t="s">
+      <c r="E18" s="172" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="86"/>
       <c r="G18" s="86"/>
-      <c r="H18" s="122" t="s">
+      <c r="H18" s="121" t="s">
         <v>196</v>
       </c>
       <c r="I18" s="89"/>
-      <c r="J18" s="166" t="s">
+      <c r="J18" s="149" t="s">
         <v>199</v>
       </c>
-      <c r="K18" s="161" t="s">
+      <c r="K18" s="144" t="s">
         <v>89</v>
       </c>
-      <c r="L18" s="161" t="s">
+      <c r="L18" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="M18" s="161" t="s">
+      <c r="M18" s="144" t="s">
         <v>130</v>
       </c>
-      <c r="N18" s="162" t="s">
+      <c r="N18" s="145" t="s">
         <v>139</v>
       </c>
       <c r="O18" s="89"/>
@@ -5438,15 +5556,15 @@
       </c>
       <c r="F19" s="86"/>
       <c r="G19" s="86"/>
-      <c r="H19" s="122"/>
+      <c r="H19" s="121"/>
       <c r="I19" s="89"/>
-      <c r="J19" s="163" t="s">
+      <c r="J19" s="146" t="s">
         <v>129</v>
       </c>
-      <c r="K19" s="157"/>
-      <c r="L19" s="157"/>
-      <c r="M19" s="157"/>
-      <c r="N19" s="164"/>
+      <c r="K19" s="140"/>
+      <c r="L19" s="140"/>
+      <c r="M19" s="140"/>
+      <c r="N19" s="147"/>
       <c r="O19" s="89"/>
     </row>
     <row r="20" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5467,17 +5585,17 @@
       </c>
       <c r="F20" s="86"/>
       <c r="G20" s="86"/>
-      <c r="H20" s="122" t="s">
+      <c r="H20" s="121" t="s">
         <v>197</v>
       </c>
       <c r="I20" s="89"/>
-      <c r="J20" s="165" t="s">
+      <c r="J20" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="157"/>
-      <c r="L20" s="157"/>
-      <c r="M20" s="157"/>
-      <c r="N20" s="164"/>
+      <c r="K20" s="140"/>
+      <c r="L20" s="140"/>
+      <c r="M20" s="140"/>
+      <c r="N20" s="147"/>
       <c r="O20" s="89"/>
     </row>
     <row r="21" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5498,17 +5616,17 @@
         <v>163</v>
       </c>
       <c r="G21" s="86"/>
-      <c r="H21" s="122" t="s">
+      <c r="H21" s="121" t="s">
         <v>137</v>
       </c>
       <c r="I21" s="89"/>
-      <c r="J21" s="167" t="s">
+      <c r="J21" s="150" t="s">
         <v>59</v>
       </c>
-      <c r="K21" s="168"/>
-      <c r="L21" s="168"/>
-      <c r="M21" s="168"/>
-      <c r="N21" s="169"/>
+      <c r="K21" s="151"/>
+      <c r="L21" s="151"/>
+      <c r="M21" s="151"/>
+      <c r="N21" s="152"/>
       <c r="O21" s="89"/>
     </row>
     <row r="22" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5529,22 +5647,22 @@
       </c>
       <c r="F22" s="86"/>
       <c r="G22" s="86"/>
-      <c r="H22" s="122"/>
+      <c r="H22" s="121"/>
       <c r="I22" s="89"/>
-      <c r="J22" s="170"/>
-      <c r="K22" s="171">
+      <c r="J22" s="153"/>
+      <c r="K22" s="154">
         <f t="shared" ref="K22:L22" si="4">SUM(K19:K21)</f>
         <v>0</v>
       </c>
-      <c r="L22" s="171">
+      <c r="L22" s="154">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M22" s="171">
+      <c r="M22" s="154">
         <f>SUM(M19:M21)</f>
         <v>0</v>
       </c>
-      <c r="N22" s="172">
+      <c r="N22" s="155">
         <f>SUM(N19:N21)</f>
         <v>0</v>
       </c>
@@ -5568,7 +5686,7 @@
       </c>
       <c r="F23" s="87"/>
       <c r="G23" s="87"/>
-      <c r="H23" s="124"/>
+      <c r="H23" s="123"/>
       <c r="I23" s="89"/>
       <c r="J23" s="89"/>
       <c r="K23" s="89"/>
@@ -5585,7 +5703,7 @@
       <c r="E24" s="83"/>
       <c r="F24" s="83"/>
       <c r="G24" s="83"/>
-      <c r="H24" s="126"/>
+      <c r="H24" s="125"/>
       <c r="I24" s="89"/>
       <c r="J24" s="89"/>
       <c r="L24" s="89"/>
@@ -5610,10 +5728,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24F838E-581A-4053-8853-3FD311356AFD}">
-  <dimension ref="B2:G49"/>
+  <dimension ref="B2:G60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5625,10 +5743,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="115" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="116"/>
+      <c r="C2" s="115"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="93" t="s">
@@ -5720,7 +5838,7 @@
       <c r="B13" s="93" t="s">
         <v>192</v>
       </c>
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="114" t="s">
         <v>152</v>
       </c>
       <c r="D13">
@@ -5747,17 +5865,17 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="118" t="s">
+      <c r="B16" s="117" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="117" t="s">
+      <c r="C16" s="116" t="s">
         <v>155</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="78"/>
     </row>
     <row r="18" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="115"/>
+      <c r="B18" s="114"/>
       <c r="C18" s="96" t="s">
         <v>193</v>
       </c>
@@ -5805,13 +5923,13 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="132" t="s">
+      <c r="B31" s="131" t="s">
         <v>172</v>
       </c>
-      <c r="C31" s="133" t="s">
+      <c r="C31" s="132" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="134"/>
+      <c r="D31" s="133"/>
     </row>
     <row r="32" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C32" s="96" t="s">
@@ -5834,19 +5952,19 @@
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="135"/>
-      <c r="C36" s="136"/>
-      <c r="D36" s="137"/>
+      <c r="B36" s="134"/>
+      <c r="C36" s="135"/>
+      <c r="D36" s="136"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="132" t="s">
+      <c r="B38" s="131" t="s">
         <v>174</v>
       </c>
-      <c r="C38" s="138" t="s">
+      <c r="C38" s="137" t="s">
         <v>175</v>
       </c>
-      <c r="D38" s="134"/>
-      <c r="E38" s="134"/>
+      <c r="D38" s="133"/>
+      <c r="E38" s="133"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C39" s="95" t="s">
@@ -5859,18 +5977,18 @@
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="139"/>
-      <c r="C41" s="136" t="s">
+      <c r="B41" s="138"/>
+      <c r="C41" s="135" t="s">
         <v>177</v>
       </c>
-      <c r="D41" s="137"/>
-      <c r="E41" s="137"/>
+      <c r="D41" s="136"/>
+      <c r="E41" s="136"/>
     </row>
     <row r="43" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B43" s="132" t="s">
+      <c r="B43" s="131" t="s">
         <v>182</v>
       </c>
-      <c r="C43" s="138" t="s">
+      <c r="C43" s="137" t="s">
         <v>183</v>
       </c>
     </row>
@@ -5880,10 +5998,10 @@
       </c>
     </row>
     <row r="46" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B46" s="138" t="s">
+      <c r="B46" s="137" t="s">
         <v>181</v>
       </c>
-      <c r="C46" s="138" t="s">
+      <c r="C46" s="137" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5893,12 +6011,64 @@
       </c>
     </row>
     <row r="49" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B49" s="135" t="s">
+      <c r="B49" s="134" t="s">
         <v>188</v>
       </c>
-      <c r="C49" s="136" t="s">
+      <c r="C49" s="135" t="s">
         <v>198</v>
       </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="95" t="s">
+        <v>200</v>
+      </c>
+      <c r="C51" s="178" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B52" s="78" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="96" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="95" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="95" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="C55" s="96" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B57" s="95" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="179" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="95" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C59" s="96" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6409,8 +6579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55CCE9F-712C-4507-AED0-56401ED0B51C}">
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7165,19 +7335,19 @@
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="141" t="s">
+      <c r="A7" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="143">
+      <c r="B7" s="159">
         <v>1</v>
       </c>
-      <c r="C7" s="145" t="s">
+      <c r="C7" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="147" t="s">
+      <c r="D7" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="149" t="s">
+      <c r="E7" s="165" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="26" t="s">
@@ -7185,11 +7355,11 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="142"/>
-      <c r="B8" s="144"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="148"/>
-      <c r="E8" s="150"/>
+      <c r="A8" s="167"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="171"/>
       <c r="F8" s="27" t="s">
         <v>40</v>
       </c>
@@ -7215,19 +7385,19 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="141" t="s">
+      <c r="A10" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="143">
+      <c r="B10" s="159">
         <v>3</v>
       </c>
-      <c r="C10" s="145" t="s">
+      <c r="C10" s="161" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="147" t="s">
+      <c r="D10" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="147" t="s">
+      <c r="E10" s="163" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="26" t="s">
@@ -7235,29 +7405,29 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="142"/>
-      <c r="B11" s="144"/>
-      <c r="C11" s="146"/>
-      <c r="D11" s="148"/>
-      <c r="E11" s="148"/>
+      <c r="A11" s="167"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="170"/>
+      <c r="E11" s="170"/>
       <c r="F11" s="21" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="141" t="s">
+      <c r="A12" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="143">
+      <c r="B12" s="159">
         <v>4</v>
       </c>
-      <c r="C12" s="145" t="s">
+      <c r="C12" s="161" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="147" t="s">
+      <c r="D12" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="147" t="s">
+      <c r="E12" s="163" t="s">
         <v>49</v>
       </c>
       <c r="F12" s="26" t="s">
@@ -7265,29 +7435,29 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="142"/>
-      <c r="B13" s="144"/>
-      <c r="C13" s="146"/>
-      <c r="D13" s="148"/>
-      <c r="E13" s="148"/>
+      <c r="A13" s="167"/>
+      <c r="B13" s="168"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="170"/>
+      <c r="E13" s="170"/>
       <c r="F13" s="21" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="141" t="s">
+      <c r="A14" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="143">
+      <c r="B14" s="159">
         <v>5</v>
       </c>
-      <c r="C14" s="145" t="s">
+      <c r="C14" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="147" t="s">
+      <c r="D14" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="147" t="s">
+      <c r="E14" s="163" t="s">
         <v>53</v>
       </c>
       <c r="F14" s="26" t="s">
@@ -7295,29 +7465,29 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="142"/>
-      <c r="B15" s="144"/>
-      <c r="C15" s="146"/>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148"/>
+      <c r="A15" s="167"/>
+      <c r="B15" s="168"/>
+      <c r="C15" s="169"/>
+      <c r="D15" s="170"/>
+      <c r="E15" s="170"/>
       <c r="F15" s="27" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="141" t="s">
+      <c r="A16" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="143">
+      <c r="B16" s="159">
         <v>6</v>
       </c>
-      <c r="C16" s="145" t="s">
+      <c r="C16" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="147" t="s">
+      <c r="D16" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="149" t="s">
+      <c r="E16" s="165" t="s">
         <v>38</v>
       </c>
       <c r="F16" s="30" t="s">
@@ -7325,11 +7495,11 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="151"/>
-      <c r="B17" s="152"/>
-      <c r="C17" s="153"/>
-      <c r="D17" s="154"/>
-      <c r="E17" s="155"/>
+      <c r="A17" s="158"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="162"/>
+      <c r="D17" s="164"/>
+      <c r="E17" s="166"/>
       <c r="F17" s="31" t="s">
         <v>58</v>
       </c>
@@ -7569,31 +7739,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>